<commit_message>
nova atualização da APS
</commit_message>
<xml_diff>
--- a/report/acs.xlsx
+++ b/report/acs.xlsx
@@ -7679,6 +7679,768 @@
     <t xml:space="preserve">27/09/1964</t>
   </si>
   <si>
+    <t xml:space="preserve">2900231</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOSSA SENHORA APARECIDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US Nossa Senhora Aparecida - GDNEB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FABRICIO FIGUEIRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6/5/2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">231</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71330496000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12516418126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GREICE DEMETRIO SANTANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/14/2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98168053087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12678260714</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANA KELLY DE ARAUJO BASTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6/3/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70503362034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12446758152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900848</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALINE FELICIANO NUNES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/21/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">848</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98733974004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12703005719</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GISELE PADILHA RIBEIRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81477171053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12929300703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18/04/1982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JANETE PEREIRA SILVEIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47502207015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12027089766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/05/1967</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARIA MARGARETE JASKULSKI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50424378000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12064109694</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/01/1966</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROSANA APARECIDA PIRES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45967636072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12309744206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19/12/1965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900486</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JORGETE MARIA FEIJO PEREIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">486</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42296986072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10878315915</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/03/1966</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2902118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VANESSA DUARTE MOREIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00615895000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12766642678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14/07/1985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAZARE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US Nazaré - GDNHNI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANGELICA MICHELE DA SILVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4/10/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00821388002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20685616112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MORRO DOS SARGENTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US Morro dos Sargentos - GDSCS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARILDE DE OLIVEIRA BUENO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76350541049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12590676680</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARTA BITTENCOURT BARCELLOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/1/2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">97744719034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12898162673</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARINES VAZ WOLMANN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3/2/2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55661491034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12272876341</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELINARA FAGUNDES MUNHOZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/17/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91454778091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20116604616</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900674</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JAQUELINE FAGUNDES HARTWIG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">674</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02592303081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13121633715</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DARCILLA PINHEIRO CAMPOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">89179579000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12580778707</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 (1 maior)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18/06/1977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROSANI TERESINHA PINTO DA SILVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73026611034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12024503316</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/10/1959</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2901765</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VANESSA ROCHA MACIEL OLIVEIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1765</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00793287090</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16045953356</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2901105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CELIA REGINA CAMPOS COSTA DE SOUZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71483349004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12406529411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900465</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MORRO DA CRUZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US Morro da Cruz - GDPLP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRASIELE REGINA CENTENO PATRICIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/24/2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">465</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02242221043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21055837703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900579</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEDIA DEISE DA SILVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/10/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">579</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48818410091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12331468852</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2901183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CATARINA DORNELLES GONCALVES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/15/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00886014042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12969224676</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2901205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALEXSANDRO SILVA DA SILVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4/6/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74795988072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12589094681</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2901180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADRIANA ROSA DA SILVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63270137087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12453241887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21/10/1974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLAUDIA RAQUEL IDALGO DE FARIAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">92157033068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19018962263</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/06/1975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2901434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRANCESCA CARLA CENTENO PATRICIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80419151087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12634529718</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25/11/1980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2901196</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GISLAINE ALVES DA COSTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1196</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90577655000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12521958389</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/06/1978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2903697</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARISTELA GIACOMINI CASTRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3697</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74820052004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12599603694</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13/08/1977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2901760</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUELI TERESINHA DA SILVA SANTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1760</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88336913068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20393112130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17/07/1965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MORADAS DA HIPICA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US Moradas da Hípica - GDSCS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLEITON SANTOS DOS PASSOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6/2/2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43626637034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10861459404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2900021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUCIANE CARDOSO THOME FRANCISCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/25/2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58371834004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12272768476</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2901212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMADEU PIO DE ALMEIDA NETO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/15/2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">92888852004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12614398677</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2901214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAISY DE LIMA BARRES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76458695004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12484045230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/01/1977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2901785</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HILDA NARA RIBEIRO SULZBACH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1785</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62724070097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12433174254</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 maiores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14/12/1971</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2902391</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IVONETE APARECIDA DOS SANTOS OLIVEIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2391</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54310008020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12511288941</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16/08/1964</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2902366</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KELLY LUCAS ARAUJO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2366</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90885171004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12560264503</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/08/1975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2902385</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LETICIA SANT ANNA CANTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2385</t>
+  </si>
+  <si>
+    <t xml:space="preserve">97130443049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12871137686</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13/04/1981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2901354</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROSEMERI MENEZES FONTES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1354</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49191586020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12294604557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30/09/1967</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2901386</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANGELA MARIA DE SOUZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/6/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1386</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96961899072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12834019713</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2901773</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VERA REGINA FRAGA CONTESSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1773</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31577474015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10850058373</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24/03/1960</t>
+  </si>
+  <si>
     <t xml:space="preserve">2900182</t>
   </si>
   <si>
@@ -7695,768 +8457,6 @@
   </si>
   <si>
     <t xml:space="preserve">02/02/1976</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900231</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOSSA SENHORA APARECIDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US Nossa Senhora Aparecida - GDNEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FABRICIO FIGUEIRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6/5/2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">231</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71330496000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12516418126</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900245</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GREICE DEMETRIO SANTANA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/14/2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">245</t>
-  </si>
-  <si>
-    <t xml:space="preserve">98168053087</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12678260714</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900809</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANA KELLY DE ARAUJO BASTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6/3/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">809</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70503362034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12446758152</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900848</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALINE FELICIANO NUNES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7/21/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">848</t>
-  </si>
-  <si>
-    <t xml:space="preserve">98733974004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12703005719</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900249</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GISELE PADILHA RIBEIRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">249</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81477171053</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12929300703</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18/04/1982</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900250</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JANETE PEREIRA SILVEIRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">250</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47502207015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12027089766</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/05/1967</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900248</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARIA MARGARETE JASKULSKI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">248</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50424378000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12064109694</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/01/1966</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROSANA APARECIDA PIRES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45967636072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12309744206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19/12/1965</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900486</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JORGETE MARIA FEIJO PEREIRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">486</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42296986072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10878315915</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07/03/1966</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2902118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VANESSA DUARTE MOREIRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00615895000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12766642678</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14/07/1985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900079</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAZARE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US Nazaré - GDNHNI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANGELICA MICHELE DA SILVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4/10/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00821388002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20685616112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MORRO DOS SARGENTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US Morro dos Sargentos - GDSCS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARILDE DE OLIVEIRA BUENO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76350541049</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12590676680</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARTA BITTENCOURT BARCELLOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/1/2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">97744719034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12898162673</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARINES VAZ WOLMANN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3/2/2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55661491034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12272876341</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELINARA FAGUNDES MUNHOZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7/17/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">91454778091</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20116604616</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900674</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JAQUELINE FAGUNDES HARTWIG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">674</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02592303081</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13121633715</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DARCILLA PINHEIRO CAMPOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">89179579000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12580778707</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 (1 maior)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18/06/1977</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROSANI TERESINHA PINTO DA SILVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73026611034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12024503316</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/10/1959</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2901765</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VANESSA ROCHA MACIEL OLIVEIRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1765</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00793287090</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16045953356</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2901105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CELIA REGINA CAMPOS COSTA DE SOUZA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71483349004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12406529411</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900465</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MORRO DA CRUZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US Morro da Cruz - GDPLP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRASIELE REGINA CENTENO PATRICIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7/24/2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">465</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02242221043</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21055837703</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900579</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEDIA DEISE DA SILVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/10/2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">579</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48818410091</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12331468852</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2901183</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CATARINA DORNELLES GONCALVES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/15/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1183</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00886014042</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12969224676</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2901205</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALEXSANDRO SILVA DA SILVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4/6/2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1205</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74795988072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12589094681</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2901180</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADRIANA ROSA DA SILVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1180</t>
-  </si>
-  <si>
-    <t xml:space="preserve">63270137087</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12453241887</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21/10/1974</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900568</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLAUDIA RAQUEL IDALGO DE FARIAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">568</t>
-  </si>
-  <si>
-    <t xml:space="preserve">92157033068</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19018962263</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/06/1975</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2901434</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FRANCESCA CARLA CENTENO PATRICIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1434</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80419151087</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12634529718</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25/11/1980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2901196</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GISLAINE ALVES DA COSTA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1196</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90577655000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12521958389</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/06/1978</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2903697</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARISTELA GIACOMINI CASTRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3697</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74820052004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12599603694</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13/08/1977</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2901760</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUELI TERESINHA DA SILVA SANTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1760</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88336913068</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20393112130</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17/07/1965</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MORADAS DA HIPICA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US Moradas da Hípica - GDSCS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GLEITON SANTOS DOS PASSOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6/2/2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43626637034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10861459404</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2900021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LUCIANE CARDOSO THOME FRANCISCO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5/25/2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58371834004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12272768476</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2901212</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMADEU PIO DE ALMEIDA NETO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8/15/2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1212</t>
-  </si>
-  <si>
-    <t xml:space="preserve">92888852004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12614398677</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2901214</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAISY DE LIMA BARRES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1214</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76458695004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12484045230</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12/01/1977</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2901785</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HILDA NARA RIBEIRO SULZBACH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1785</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62724070097</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12433174254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 maiores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14/12/1971</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2902391</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IVONETE APARECIDA DOS SANTOS OLIVEIRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2391</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54310008020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12511288941</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16/08/1964</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2902366</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KELLY LUCAS ARAUJO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2366</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90885171004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12560264503</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03/08/1975</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2902385</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LETICIA SANT ANNA CANTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2385</t>
-  </si>
-  <si>
-    <t xml:space="preserve">97130443049</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12871137686</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13/04/1981</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2901354</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROSEMERI MENEZES FONTES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1354</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49191586020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12294604557</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30/09/1967</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2901386</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANGELA MARIA DE SOUZA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5/6/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1386</t>
-  </si>
-  <si>
-    <t xml:space="preserve">96961899072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12834019713</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2901773</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VERA REGINA FRAGA CONTESSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1773</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31577474015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10850058373</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24/03/1960</t>
   </si>
   <si>
     <t xml:space="preserve">2901456</t>
@@ -25961,7 +25961,7 @@
         <v>22529</v>
       </c>
       <c r="U112" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="113">
@@ -34251,7 +34251,7 @@
         <v>32022</v>
       </c>
       <c r="U254" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="255">
@@ -42999,41 +42999,41 @@
         <v>2555</v>
       </c>
       <c r="B405" t="s">
-        <v>2507</v>
+        <v>2556</v>
       </c>
       <c r="C405" t="s">
-        <v>2508</v>
+        <v>2557</v>
       </c>
       <c r="D405" t="s">
-        <v>2556</v>
+        <v>2558</v>
       </c>
       <c r="E405"/>
       <c r="F405" t="s">
-        <v>66</v>
+        <v>2559</v>
       </c>
       <c r="G405" t="s">
-        <v>2557</v>
+        <v>2560</v>
       </c>
       <c r="H405" s="1" t="n">
-        <v>40954</v>
+        <v>40953</v>
       </c>
       <c r="I405" t="s">
         <v>27</v>
       </c>
       <c r="J405" t="s">
-        <v>2558</v>
+        <v>2561</v>
       </c>
       <c r="K405" t="s">
-        <v>2559</v>
+        <v>2562</v>
       </c>
       <c r="L405" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="M405" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N405" t="s">
-        <v>2560</v>
+        <v>32</v>
       </c>
       <c r="O405" t="s">
         <v>33</v>
@@ -43046,24 +43046,20 @@
       </c>
       <c r="R405"/>
       <c r="S405" t="b">
-        <v>1</v>
-      </c>
-      <c r="T405" s="1" t="n">
-        <v>27792</v>
-      </c>
-      <c r="U405" t="n">
-        <v>45</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T405" s="1"/>
+      <c r="U405"/>
     </row>
     <row r="406">
       <c r="A406" t="s">
-        <v>2561</v>
+        <v>2563</v>
       </c>
       <c r="B406" t="s">
-        <v>2562</v>
+        <v>2556</v>
       </c>
       <c r="C406" t="s">
-        <v>2563</v>
+        <v>2557</v>
       </c>
       <c r="D406" t="s">
         <v>2564</v>
@@ -43076,7 +43072,7 @@
         <v>2566</v>
       </c>
       <c r="H406" s="1" t="n">
-        <v>40953</v>
+        <v>40940</v>
       </c>
       <c r="I406" t="s">
         <v>27</v>
@@ -43088,7 +43084,7 @@
         <v>2568</v>
       </c>
       <c r="L406" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="M406" t="s">
         <v>31</v>
@@ -43117,10 +43113,10 @@
         <v>2569</v>
       </c>
       <c r="B407" t="s">
-        <v>2562</v>
+        <v>2556</v>
       </c>
       <c r="C407" t="s">
-        <v>2563</v>
+        <v>2557</v>
       </c>
       <c r="D407" t="s">
         <v>2570</v>
@@ -43133,7 +43129,7 @@
         <v>2572</v>
       </c>
       <c r="H407" s="1" t="n">
-        <v>40940</v>
+        <v>41218</v>
       </c>
       <c r="I407" t="s">
         <v>27</v>
@@ -43145,7 +43141,7 @@
         <v>2574</v>
       </c>
       <c r="L407" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="M407" t="s">
         <v>31</v>
@@ -43174,10 +43170,10 @@
         <v>2575</v>
       </c>
       <c r="B408" t="s">
-        <v>2562</v>
+        <v>2556</v>
       </c>
       <c r="C408" t="s">
-        <v>2563</v>
+        <v>2557</v>
       </c>
       <c r="D408" t="s">
         <v>2576</v>
@@ -43190,7 +43186,7 @@
         <v>2578</v>
       </c>
       <c r="H408" s="1" t="n">
-        <v>41218</v>
+        <v>41226</v>
       </c>
       <c r="I408" t="s">
         <v>27</v>
@@ -43202,7 +43198,7 @@
         <v>2580</v>
       </c>
       <c r="L408" t="s">
-        <v>47</v>
+        <v>519</v>
       </c>
       <c r="M408" t="s">
         <v>31</v>
@@ -43231,41 +43227,41 @@
         <v>2581</v>
       </c>
       <c r="B409" t="s">
-        <v>2562</v>
+        <v>2556</v>
       </c>
       <c r="C409" t="s">
-        <v>2563</v>
+        <v>2557</v>
       </c>
       <c r="D409" t="s">
         <v>2582</v>
       </c>
       <c r="E409"/>
       <c r="F409" t="s">
+        <v>66</v>
+      </c>
+      <c r="G409" t="s">
         <v>2583</v>
       </c>
-      <c r="G409" t="s">
+      <c r="H409" s="1" t="n">
+        <v>40940</v>
+      </c>
+      <c r="I409" t="s">
+        <v>27</v>
+      </c>
+      <c r="J409" t="s">
         <v>2584</v>
       </c>
-      <c r="H409" s="1" t="n">
-        <v>41226</v>
-      </c>
-      <c r="I409" t="s">
-        <v>27</v>
-      </c>
-      <c r="J409" t="s">
+      <c r="K409" t="s">
         <v>2585</v>
       </c>
-      <c r="K409" t="s">
+      <c r="L409" t="s">
+        <v>47</v>
+      </c>
+      <c r="M409" t="s">
+        <v>479</v>
+      </c>
+      <c r="N409" t="s">
         <v>2586</v>
-      </c>
-      <c r="L409" t="s">
-        <v>519</v>
-      </c>
-      <c r="M409" t="s">
-        <v>31</v>
-      </c>
-      <c r="N409" t="s">
-        <v>32</v>
       </c>
       <c r="O409" t="s">
         <v>33</v>
@@ -43278,20 +43274,24 @@
       </c>
       <c r="R409"/>
       <c r="S409" t="b">
-        <v>0</v>
-      </c>
-      <c r="T409" s="1"/>
-      <c r="U409"/>
+        <v>1</v>
+      </c>
+      <c r="T409" s="1" t="n">
+        <v>30059</v>
+      </c>
+      <c r="U409" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="410">
       <c r="A410" t="s">
         <v>2587</v>
       </c>
       <c r="B410" t="s">
-        <v>2562</v>
+        <v>2556</v>
       </c>
       <c r="C410" t="s">
-        <v>2563</v>
+        <v>2557</v>
       </c>
       <c r="D410" t="s">
         <v>2588</v>
@@ -43304,7 +43304,7 @@
         <v>2589</v>
       </c>
       <c r="H410" s="1" t="n">
-        <v>40940</v>
+        <v>40947</v>
       </c>
       <c r="I410" t="s">
         <v>27</v>
@@ -43319,7 +43319,7 @@
         <v>47</v>
       </c>
       <c r="M410" t="s">
-        <v>479</v>
+        <v>55</v>
       </c>
       <c r="N410" t="s">
         <v>2592</v>
@@ -43338,10 +43338,10 @@
         <v>1</v>
       </c>
       <c r="T410" s="1" t="n">
-        <v>30059</v>
+        <v>24603</v>
       </c>
       <c r="U410" t="n">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="411">
@@ -43349,10 +43349,10 @@
         <v>2593</v>
       </c>
       <c r="B411" t="s">
-        <v>2562</v>
+        <v>2556</v>
       </c>
       <c r="C411" t="s">
-        <v>2563</v>
+        <v>2557</v>
       </c>
       <c r="D411" t="s">
         <v>2594</v>
@@ -43365,7 +43365,7 @@
         <v>2595</v>
       </c>
       <c r="H411" s="1" t="n">
-        <v>40947</v>
+        <v>40940</v>
       </c>
       <c r="I411" t="s">
         <v>27</v>
@@ -43399,10 +43399,10 @@
         <v>1</v>
       </c>
       <c r="T411" s="1" t="n">
-        <v>24603</v>
+        <v>24116</v>
       </c>
       <c r="U411" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="412">
@@ -43410,10 +43410,10 @@
         <v>2599</v>
       </c>
       <c r="B412" t="s">
-        <v>2562</v>
+        <v>2556</v>
       </c>
       <c r="C412" t="s">
-        <v>2563</v>
+        <v>2557</v>
       </c>
       <c r="D412" t="s">
         <v>2600</v>
@@ -43460,7 +43460,7 @@
         <v>1</v>
       </c>
       <c r="T412" s="1" t="n">
-        <v>24116</v>
+        <v>24095</v>
       </c>
       <c r="U412" t="n">
         <v>55</v>
@@ -43471,23 +43471,21 @@
         <v>2605</v>
       </c>
       <c r="B413" t="s">
-        <v>2562</v>
+        <v>2556</v>
       </c>
       <c r="C413" t="s">
-        <v>2563</v>
+        <v>2557</v>
       </c>
       <c r="D413" t="s">
         <v>2606</v>
       </c>
       <c r="E413"/>
-      <c r="F413" t="s">
-        <v>66</v>
-      </c>
+      <c r="F413"/>
       <c r="G413" t="s">
         <v>2607</v>
       </c>
       <c r="H413" s="1" t="n">
-        <v>40940</v>
+        <v>41171</v>
       </c>
       <c r="I413" t="s">
         <v>27</v>
@@ -43521,7 +43519,7 @@
         <v>1</v>
       </c>
       <c r="T413" s="1" t="n">
-        <v>24095</v>
+        <v>24173</v>
       </c>
       <c r="U413" t="n">
         <v>55</v>
@@ -43532,10 +43530,10 @@
         <v>2611</v>
       </c>
       <c r="B414" t="s">
-        <v>2562</v>
+        <v>2556</v>
       </c>
       <c r="C414" t="s">
-        <v>2563</v>
+        <v>2557</v>
       </c>
       <c r="D414" t="s">
         <v>2612</v>
@@ -43546,7 +43544,7 @@
         <v>2613</v>
       </c>
       <c r="H414" s="1" t="n">
-        <v>41171</v>
+        <v>41709</v>
       </c>
       <c r="I414" t="s">
         <v>27</v>
@@ -43580,10 +43578,10 @@
         <v>1</v>
       </c>
       <c r="T414" s="1" t="n">
-        <v>24173</v>
+        <v>31242</v>
       </c>
       <c r="U414" t="n">
-        <v>55</v>
+        <v>36</v>
       </c>
     </row>
     <row r="415">
@@ -43591,39 +43589,41 @@
         <v>2617</v>
       </c>
       <c r="B415" t="s">
-        <v>2562</v>
+        <v>2618</v>
       </c>
       <c r="C415" t="s">
-        <v>2563</v>
+        <v>2619</v>
       </c>
       <c r="D415" t="s">
-        <v>2618</v>
+        <v>2620</v>
       </c>
       <c r="E415"/>
-      <c r="F415"/>
+      <c r="F415" t="s">
+        <v>2621</v>
+      </c>
       <c r="G415" t="s">
-        <v>2619</v>
+        <v>2622</v>
       </c>
       <c r="H415" s="1" t="n">
-        <v>41709</v>
+        <v>40940</v>
       </c>
       <c r="I415" t="s">
         <v>27</v>
       </c>
       <c r="J415" t="s">
-        <v>2620</v>
+        <v>2623</v>
       </c>
       <c r="K415" t="s">
-        <v>2621</v>
+        <v>2624</v>
       </c>
       <c r="L415" t="s">
         <v>47</v>
       </c>
       <c r="M415" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="N415" t="s">
-        <v>2622</v>
+        <v>32</v>
       </c>
       <c r="O415" t="s">
         <v>33</v>
@@ -43636,34 +43636,30 @@
       </c>
       <c r="R415"/>
       <c r="S415" t="b">
-        <v>1</v>
-      </c>
-      <c r="T415" s="1" t="n">
-        <v>31242</v>
-      </c>
-      <c r="U415" t="n">
-        <v>36</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T415" s="1"/>
+      <c r="U415"/>
     </row>
     <row r="416">
       <c r="A416" t="s">
-        <v>2623</v>
+        <v>2625</v>
       </c>
       <c r="B416" t="s">
-        <v>2624</v>
+        <v>2626</v>
       </c>
       <c r="C416" t="s">
-        <v>2625</v>
+        <v>2627</v>
       </c>
       <c r="D416" t="s">
-        <v>2626</v>
+        <v>2628</v>
       </c>
       <c r="E416"/>
       <c r="F416" t="s">
-        <v>2627</v>
+        <v>109</v>
       </c>
       <c r="G416" t="s">
-        <v>2628</v>
+        <v>2629</v>
       </c>
       <c r="H416" s="1" t="n">
         <v>40940</v>
@@ -43672,10 +43668,10 @@
         <v>27</v>
       </c>
       <c r="J416" t="s">
-        <v>2629</v>
+        <v>2630</v>
       </c>
       <c r="K416" t="s">
-        <v>2630</v>
+        <v>2631</v>
       </c>
       <c r="L416" t="s">
         <v>47</v>
@@ -43704,20 +43700,20 @@
     </row>
     <row r="417">
       <c r="A417" t="s">
-        <v>2631</v>
+        <v>2632</v>
       </c>
       <c r="B417" t="s">
-        <v>2632</v>
+        <v>2626</v>
       </c>
       <c r="C417" t="s">
+        <v>2627</v>
+      </c>
+      <c r="D417" t="s">
         <v>2633</v>
-      </c>
-      <c r="D417" t="s">
-        <v>2634</v>
       </c>
       <c r="E417"/>
       <c r="F417" t="s">
-        <v>109</v>
+        <v>2634</v>
       </c>
       <c r="G417" t="s">
         <v>2635</v>
@@ -43735,7 +43731,7 @@
         <v>2637</v>
       </c>
       <c r="L417" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="M417" t="s">
         <v>31</v>
@@ -43764,10 +43760,10 @@
         <v>2638</v>
       </c>
       <c r="B418" t="s">
-        <v>2632</v>
+        <v>2626</v>
       </c>
       <c r="C418" t="s">
-        <v>2633</v>
+        <v>2627</v>
       </c>
       <c r="D418" t="s">
         <v>2639</v>
@@ -43792,7 +43788,7 @@
         <v>2643</v>
       </c>
       <c r="L418" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="M418" t="s">
         <v>31</v>
@@ -43821,10 +43817,10 @@
         <v>2644</v>
       </c>
       <c r="B419" t="s">
-        <v>2632</v>
+        <v>2626</v>
       </c>
       <c r="C419" t="s">
-        <v>2633</v>
+        <v>2627</v>
       </c>
       <c r="D419" t="s">
         <v>2645</v>
@@ -43849,7 +43845,7 @@
         <v>2649</v>
       </c>
       <c r="L419" t="s">
-        <v>99</v>
+        <v>47</v>
       </c>
       <c r="M419" t="s">
         <v>31</v>
@@ -43878,32 +43874,32 @@
         <v>2650</v>
       </c>
       <c r="B420" t="s">
-        <v>2632</v>
+        <v>2626</v>
       </c>
       <c r="C420" t="s">
-        <v>2633</v>
+        <v>2627</v>
       </c>
       <c r="D420" t="s">
         <v>2651</v>
       </c>
       <c r="E420"/>
       <c r="F420" t="s">
+        <v>2646</v>
+      </c>
+      <c r="G420" t="s">
         <v>2652</v>
       </c>
-      <c r="G420" t="s">
+      <c r="H420" s="1" t="n">
+        <v>41169</v>
+      </c>
+      <c r="I420" t="s">
+        <v>27</v>
+      </c>
+      <c r="J420" t="s">
         <v>2653</v>
       </c>
-      <c r="H420" s="1" t="n">
-        <v>40940</v>
-      </c>
-      <c r="I420" t="s">
-        <v>27</v>
-      </c>
-      <c r="J420" t="s">
+      <c r="K420" t="s">
         <v>2654</v>
-      </c>
-      <c r="K420" t="s">
-        <v>2655</v>
       </c>
       <c r="L420" t="s">
         <v>47</v>
@@ -43932,44 +43928,44 @@
     </row>
     <row r="421">
       <c r="A421" t="s">
+        <v>2655</v>
+      </c>
+      <c r="B421" t="s">
+        <v>2626</v>
+      </c>
+      <c r="C421" t="s">
+        <v>2627</v>
+      </c>
+      <c r="D421" t="s">
         <v>2656</v>
-      </c>
-      <c r="B421" t="s">
-        <v>2632</v>
-      </c>
-      <c r="C421" t="s">
-        <v>2633</v>
-      </c>
-      <c r="D421" t="s">
-        <v>2657</v>
       </c>
       <c r="E421"/>
       <c r="F421" t="s">
-        <v>2652</v>
+        <v>66</v>
       </c>
       <c r="G421" t="s">
+        <v>2657</v>
+      </c>
+      <c r="H421" s="1" t="n">
+        <v>40940</v>
+      </c>
+      <c r="I421" t="s">
+        <v>27</v>
+      </c>
+      <c r="J421" t="s">
         <v>2658</v>
       </c>
-      <c r="H421" s="1" t="n">
-        <v>41169</v>
-      </c>
-      <c r="I421" t="s">
-        <v>27</v>
-      </c>
-      <c r="J421" t="s">
+      <c r="K421" t="s">
         <v>2659</v>
-      </c>
-      <c r="K421" t="s">
-        <v>2660</v>
       </c>
       <c r="L421" t="s">
         <v>47</v>
       </c>
       <c r="M421" t="s">
-        <v>31</v>
+        <v>2660</v>
       </c>
       <c r="N421" t="s">
-        <v>32</v>
+        <v>2661</v>
       </c>
       <c r="O421" t="s">
         <v>33</v>
@@ -43982,30 +43978,34 @@
       </c>
       <c r="R421"/>
       <c r="S421" t="b">
-        <v>0</v>
-      </c>
-      <c r="T421" s="1"/>
-      <c r="U421"/>
+        <v>1</v>
+      </c>
+      <c r="T421" s="1" t="n">
+        <v>28294</v>
+      </c>
+      <c r="U421" t="n">
+        <v>44</v>
+      </c>
     </row>
     <row r="422">
       <c r="A422" t="s">
-        <v>2661</v>
+        <v>2662</v>
       </c>
       <c r="B422" t="s">
-        <v>2632</v>
+        <v>2626</v>
       </c>
       <c r="C422" t="s">
-        <v>2633</v>
+        <v>2627</v>
       </c>
       <c r="D422" t="s">
-        <v>2662</v>
+        <v>2663</v>
       </c>
       <c r="E422"/>
       <c r="F422" t="s">
         <v>66</v>
       </c>
       <c r="G422" t="s">
-        <v>2663</v>
+        <v>2664</v>
       </c>
       <c r="H422" s="1" t="n">
         <v>40940</v>
@@ -44014,16 +44014,16 @@
         <v>27</v>
       </c>
       <c r="J422" t="s">
-        <v>2664</v>
+        <v>2665</v>
       </c>
       <c r="K422" t="s">
-        <v>2665</v>
+        <v>2666</v>
       </c>
       <c r="L422" t="s">
         <v>47</v>
       </c>
       <c r="M422" t="s">
-        <v>2666</v>
+        <v>55</v>
       </c>
       <c r="N422" t="s">
         <v>2667</v>
@@ -44042,10 +44042,10 @@
         <v>1</v>
       </c>
       <c r="T422" s="1" t="n">
-        <v>28294</v>
+        <v>21832</v>
       </c>
       <c r="U422" t="n">
-        <v>44</v>
+        <v>61</v>
       </c>
     </row>
     <row r="423">
@@ -44053,23 +44053,23 @@
         <v>2668</v>
       </c>
       <c r="B423" t="s">
-        <v>2632</v>
+        <v>2626</v>
       </c>
       <c r="C423" t="s">
-        <v>2633</v>
+        <v>2627</v>
       </c>
       <c r="D423" t="s">
         <v>2669</v>
       </c>
       <c r="E423"/>
       <c r="F423" t="s">
-        <v>66</v>
+        <v>1286</v>
       </c>
       <c r="G423" t="s">
         <v>2670</v>
       </c>
       <c r="H423" s="1" t="n">
-        <v>40940</v>
+        <v>41554</v>
       </c>
       <c r="I423" t="s">
         <v>27</v>
@@ -44084,10 +44084,10 @@
         <v>47</v>
       </c>
       <c r="M423" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="N423" t="s">
-        <v>2673</v>
+        <v>32</v>
       </c>
       <c r="O423" t="s">
         <v>33</v>
@@ -44100,55 +44100,49 @@
       </c>
       <c r="R423"/>
       <c r="S423" t="b">
-        <v>1</v>
-      </c>
-      <c r="T423" s="1" t="n">
-        <v>21832</v>
-      </c>
-      <c r="U423" t="n">
-        <v>61</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T423" s="1"/>
+      <c r="U423"/>
     </row>
     <row r="424">
       <c r="A424" t="s">
+        <v>2673</v>
+      </c>
+      <c r="B424" t="s">
+        <v>2626</v>
+      </c>
+      <c r="C424" t="s">
+        <v>2627</v>
+      </c>
+      <c r="D424" t="s">
         <v>2674</v>
       </c>
-      <c r="B424" t="s">
-        <v>2632</v>
-      </c>
-      <c r="C424" t="s">
-        <v>2633</v>
-      </c>
-      <c r="D424" t="s">
+      <c r="E424"/>
+      <c r="F424"/>
+      <c r="G424" t="s">
         <v>2675</v>
       </c>
-      <c r="E424"/>
-      <c r="F424" t="s">
-        <v>1286</v>
-      </c>
-      <c r="G424" t="s">
+      <c r="H424" s="1" t="n">
+        <v>41256</v>
+      </c>
+      <c r="I424" t="s">
+        <v>27</v>
+      </c>
+      <c r="J424" t="s">
         <v>2676</v>
       </c>
-      <c r="H424" s="1" t="n">
-        <v>41554</v>
-      </c>
-      <c r="I424" t="s">
-        <v>27</v>
-      </c>
-      <c r="J424" t="s">
+      <c r="K424" t="s">
         <v>2677</v>
-      </c>
-      <c r="K424" t="s">
-        <v>2678</v>
       </c>
       <c r="L424" t="s">
         <v>47</v>
       </c>
       <c r="M424" t="s">
-        <v>100</v>
+        <v>813</v>
       </c>
       <c r="N424" t="s">
-        <v>32</v>
+        <v>2010</v>
       </c>
       <c r="O424" t="s">
         <v>33</v>
@@ -44161,49 +44155,55 @@
       </c>
       <c r="R424"/>
       <c r="S424" t="b">
-        <v>0</v>
-      </c>
-      <c r="T424" s="1"/>
-      <c r="U424"/>
+        <v>1</v>
+      </c>
+      <c r="T424" s="1" t="n">
+        <v>27686</v>
+      </c>
+      <c r="U424" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="425">
       <c r="A425" t="s">
+        <v>2678</v>
+      </c>
+      <c r="B425" t="s">
         <v>2679</v>
       </c>
-      <c r="B425" t="s">
-        <v>2632</v>
-      </c>
       <c r="C425" t="s">
-        <v>2633</v>
+        <v>2680</v>
       </c>
       <c r="D425" t="s">
-        <v>2680</v>
+        <v>2681</v>
       </c>
       <c r="E425"/>
-      <c r="F425"/>
+      <c r="F425" t="s">
+        <v>2682</v>
+      </c>
       <c r="G425" t="s">
-        <v>2681</v>
+        <v>2683</v>
       </c>
       <c r="H425" s="1" t="n">
-        <v>41256</v>
+        <v>41185</v>
       </c>
       <c r="I425" t="s">
         <v>27</v>
       </c>
       <c r="J425" t="s">
-        <v>2682</v>
+        <v>2684</v>
       </c>
       <c r="K425" t="s">
-        <v>2683</v>
+        <v>2685</v>
       </c>
       <c r="L425" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="M425" t="s">
-        <v>813</v>
+        <v>31</v>
       </c>
       <c r="N425" t="s">
-        <v>2010</v>
+        <v>32</v>
       </c>
       <c r="O425" t="s">
         <v>33</v>
@@ -44216,24 +44216,20 @@
       </c>
       <c r="R425"/>
       <c r="S425" t="b">
-        <v>1</v>
-      </c>
-      <c r="T425" s="1" t="n">
-        <v>27686</v>
-      </c>
-      <c r="U425" t="n">
-        <v>45</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T425" s="1"/>
+      <c r="U425"/>
     </row>
     <row r="426">
       <c r="A426" t="s">
-        <v>2684</v>
+        <v>2686</v>
       </c>
       <c r="B426" t="s">
-        <v>2685</v>
+        <v>2679</v>
       </c>
       <c r="C426" t="s">
-        <v>2686</v>
+        <v>2680</v>
       </c>
       <c r="D426" t="s">
         <v>2687</v>
@@ -44246,7 +44242,7 @@
         <v>2689</v>
       </c>
       <c r="H426" s="1" t="n">
-        <v>41185</v>
+        <v>41334</v>
       </c>
       <c r="I426" t="s">
         <v>27</v>
@@ -44258,7 +44254,7 @@
         <v>2691</v>
       </c>
       <c r="L426" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="M426" t="s">
         <v>31</v>
@@ -44287,10 +44283,10 @@
         <v>2692</v>
       </c>
       <c r="B427" t="s">
-        <v>2685</v>
+        <v>2679</v>
       </c>
       <c r="C427" t="s">
-        <v>2686</v>
+        <v>2680</v>
       </c>
       <c r="D427" t="s">
         <v>2693</v>
@@ -44344,10 +44340,10 @@
         <v>2698</v>
       </c>
       <c r="B428" t="s">
-        <v>2685</v>
+        <v>2679</v>
       </c>
       <c r="C428" t="s">
-        <v>2686</v>
+        <v>2680</v>
       </c>
       <c r="D428" t="s">
         <v>2699</v>
@@ -44360,7 +44356,7 @@
         <v>2701</v>
       </c>
       <c r="H428" s="1" t="n">
-        <v>41334</v>
+        <v>41296</v>
       </c>
       <c r="I428" t="s">
         <v>27</v>
@@ -44401,41 +44397,39 @@
         <v>2704</v>
       </c>
       <c r="B429" t="s">
-        <v>2685</v>
+        <v>2679</v>
       </c>
       <c r="C429" t="s">
-        <v>2686</v>
+        <v>2680</v>
       </c>
       <c r="D429" t="s">
         <v>2705</v>
       </c>
       <c r="E429"/>
-      <c r="F429" t="s">
+      <c r="F429"/>
+      <c r="G429" t="s">
         <v>2706</v>
       </c>
-      <c r="G429" t="s">
+      <c r="H429" s="1" t="n">
+        <v>41386</v>
+      </c>
+      <c r="I429" t="s">
+        <v>27</v>
+      </c>
+      <c r="J429" t="s">
         <v>2707</v>
       </c>
-      <c r="H429" s="1" t="n">
-        <v>41296</v>
-      </c>
-      <c r="I429" t="s">
-        <v>27</v>
-      </c>
-      <c r="J429" t="s">
+      <c r="K429" t="s">
         <v>2708</v>
       </c>
-      <c r="K429" t="s">
+      <c r="L429" t="s">
+        <v>47</v>
+      </c>
+      <c r="M429" t="s">
+        <v>48</v>
+      </c>
+      <c r="N429" t="s">
         <v>2709</v>
-      </c>
-      <c r="L429" t="s">
-        <v>92</v>
-      </c>
-      <c r="M429" t="s">
-        <v>31</v>
-      </c>
-      <c r="N429" t="s">
-        <v>32</v>
       </c>
       <c r="O429" t="s">
         <v>33</v>
@@ -44448,20 +44442,24 @@
       </c>
       <c r="R429"/>
       <c r="S429" t="b">
-        <v>0</v>
-      </c>
-      <c r="T429" s="1"/>
-      <c r="U429"/>
+        <v>1</v>
+      </c>
+      <c r="T429" s="1" t="n">
+        <v>27323</v>
+      </c>
+      <c r="U429" t="n">
+        <v>46</v>
+      </c>
     </row>
     <row r="430">
       <c r="A430" t="s">
         <v>2710</v>
       </c>
       <c r="B430" t="s">
-        <v>2685</v>
+        <v>2679</v>
       </c>
       <c r="C430" t="s">
-        <v>2686</v>
+        <v>2680</v>
       </c>
       <c r="D430" t="s">
         <v>2711</v>
@@ -44472,7 +44470,7 @@
         <v>2712</v>
       </c>
       <c r="H430" s="1" t="n">
-        <v>41386</v>
+        <v>41176</v>
       </c>
       <c r="I430" t="s">
         <v>27</v>
@@ -44487,7 +44485,7 @@
         <v>47</v>
       </c>
       <c r="M430" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="N430" t="s">
         <v>2715</v>
@@ -44506,7 +44504,7 @@
         <v>1</v>
       </c>
       <c r="T430" s="1" t="n">
-        <v>27323</v>
+        <v>27556</v>
       </c>
       <c r="U430" t="n">
         <v>46</v>
@@ -44517,10 +44515,10 @@
         <v>2716</v>
       </c>
       <c r="B431" t="s">
-        <v>2685</v>
+        <v>2679</v>
       </c>
       <c r="C431" t="s">
-        <v>2686</v>
+        <v>2680</v>
       </c>
       <c r="D431" t="s">
         <v>2717</v>
@@ -44531,7 +44529,7 @@
         <v>2718</v>
       </c>
       <c r="H431" s="1" t="n">
-        <v>41176</v>
+        <v>41428</v>
       </c>
       <c r="I431" t="s">
         <v>27</v>
@@ -44546,7 +44544,7 @@
         <v>47</v>
       </c>
       <c r="M431" t="s">
-        <v>55</v>
+        <v>1620</v>
       </c>
       <c r="N431" t="s">
         <v>2721</v>
@@ -44565,10 +44563,10 @@
         <v>1</v>
       </c>
       <c r="T431" s="1" t="n">
-        <v>27556</v>
+        <v>29550</v>
       </c>
       <c r="U431" t="n">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="432">
@@ -44576,10 +44574,10 @@
         <v>2722</v>
       </c>
       <c r="B432" t="s">
-        <v>2685</v>
+        <v>2679</v>
       </c>
       <c r="C432" t="s">
-        <v>2686</v>
+        <v>2680</v>
       </c>
       <c r="D432" t="s">
         <v>2723</v>
@@ -44590,7 +44588,7 @@
         <v>2724</v>
       </c>
       <c r="H432" s="1" t="n">
-        <v>41428</v>
+        <v>41291</v>
       </c>
       <c r="I432" t="s">
         <v>27</v>
@@ -44605,7 +44603,7 @@
         <v>47</v>
       </c>
       <c r="M432" t="s">
-        <v>1620</v>
+        <v>70</v>
       </c>
       <c r="N432" t="s">
         <v>2727</v>
@@ -44624,10 +44622,10 @@
         <v>1</v>
       </c>
       <c r="T432" s="1" t="n">
-        <v>29550</v>
+        <v>28650</v>
       </c>
       <c r="U432" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="433">
@@ -44635,10 +44633,10 @@
         <v>2728</v>
       </c>
       <c r="B433" t="s">
-        <v>2685</v>
+        <v>2679</v>
       </c>
       <c r="C433" t="s">
-        <v>2686</v>
+        <v>2680</v>
       </c>
       <c r="D433" t="s">
         <v>2729</v>
@@ -44649,7 +44647,7 @@
         <v>2730</v>
       </c>
       <c r="H433" s="1" t="n">
-        <v>41291</v>
+        <v>43536</v>
       </c>
       <c r="I433" t="s">
         <v>27</v>
@@ -44664,7 +44662,7 @@
         <v>47</v>
       </c>
       <c r="M433" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="N433" t="s">
         <v>2733</v>
@@ -44683,10 +44681,10 @@
         <v>1</v>
       </c>
       <c r="T433" s="1" t="n">
-        <v>28650</v>
+        <v>28350</v>
       </c>
       <c r="U433" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="434">
@@ -44694,10 +44692,10 @@
         <v>2734</v>
       </c>
       <c r="B434" t="s">
-        <v>2685</v>
+        <v>2679</v>
       </c>
       <c r="C434" t="s">
-        <v>2686</v>
+        <v>2680</v>
       </c>
       <c r="D434" t="s">
         <v>2735</v>
@@ -44708,7 +44706,7 @@
         <v>2736</v>
       </c>
       <c r="H434" s="1" t="n">
-        <v>43536</v>
+        <v>41582</v>
       </c>
       <c r="I434" t="s">
         <v>27</v>
@@ -44723,7 +44721,7 @@
         <v>47</v>
       </c>
       <c r="M434" t="s">
-        <v>48</v>
+        <v>479</v>
       </c>
       <c r="N434" t="s">
         <v>2739</v>
@@ -44742,10 +44740,10 @@
         <v>1</v>
       </c>
       <c r="T434" s="1" t="n">
-        <v>28350</v>
+        <v>23940</v>
       </c>
       <c r="U434" t="n">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="435">
@@ -44753,39 +44751,41 @@
         <v>2740</v>
       </c>
       <c r="B435" t="s">
-        <v>2685</v>
+        <v>2741</v>
       </c>
       <c r="C435" t="s">
-        <v>2686</v>
+        <v>2742</v>
       </c>
       <c r="D435" t="s">
-        <v>2741</v>
+        <v>2743</v>
       </c>
       <c r="E435"/>
-      <c r="F435"/>
+      <c r="F435" t="s">
+        <v>2744</v>
+      </c>
       <c r="G435" t="s">
-        <v>2742</v>
+        <v>2745</v>
       </c>
       <c r="H435" s="1" t="n">
-        <v>41582</v>
+        <v>40940</v>
       </c>
       <c r="I435" t="s">
         <v>27</v>
       </c>
       <c r="J435" t="s">
-        <v>2743</v>
+        <v>2746</v>
       </c>
       <c r="K435" t="s">
-        <v>2744</v>
+        <v>2747</v>
       </c>
       <c r="L435" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="M435" t="s">
-        <v>479</v>
+        <v>31</v>
       </c>
       <c r="N435" t="s">
-        <v>2745</v>
+        <v>32</v>
       </c>
       <c r="O435" t="s">
         <v>33</v>
@@ -44798,24 +44798,20 @@
       </c>
       <c r="R435"/>
       <c r="S435" t="b">
-        <v>1</v>
-      </c>
-      <c r="T435" s="1" t="n">
-        <v>23940</v>
-      </c>
-      <c r="U435" t="n">
-        <v>56</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T435" s="1"/>
+      <c r="U435"/>
     </row>
     <row r="436">
       <c r="A436" t="s">
-        <v>2746</v>
+        <v>2748</v>
       </c>
       <c r="B436" t="s">
-        <v>2747</v>
+        <v>2741</v>
       </c>
       <c r="C436" t="s">
-        <v>2748</v>
+        <v>2742</v>
       </c>
       <c r="D436" t="s">
         <v>2749</v>
@@ -44840,7 +44836,7 @@
         <v>2753</v>
       </c>
       <c r="L436" t="s">
-        <v>99</v>
+        <v>170</v>
       </c>
       <c r="M436" t="s">
         <v>31</v>
@@ -44869,10 +44865,10 @@
         <v>2754</v>
       </c>
       <c r="B437" t="s">
-        <v>2747</v>
+        <v>2741</v>
       </c>
       <c r="C437" t="s">
-        <v>2748</v>
+        <v>2742</v>
       </c>
       <c r="D437" t="s">
         <v>2755</v>
@@ -44885,7 +44881,7 @@
         <v>2757</v>
       </c>
       <c r="H437" s="1" t="n">
-        <v>40940</v>
+        <v>41379</v>
       </c>
       <c r="I437" t="s">
         <v>27</v>
@@ -44897,7 +44893,7 @@
         <v>2759</v>
       </c>
       <c r="L437" t="s">
-        <v>170</v>
+        <v>30</v>
       </c>
       <c r="M437" t="s">
         <v>31</v>
@@ -44926,41 +44922,39 @@
         <v>2760</v>
       </c>
       <c r="B438" t="s">
-        <v>2747</v>
+        <v>2741</v>
       </c>
       <c r="C438" t="s">
-        <v>2748</v>
+        <v>2742</v>
       </c>
       <c r="D438" t="s">
         <v>2761</v>
       </c>
       <c r="E438"/>
-      <c r="F438" t="s">
+      <c r="F438"/>
+      <c r="G438" t="s">
         <v>2762</v>
       </c>
-      <c r="G438" t="s">
+      <c r="H438" s="1" t="n">
+        <v>41295</v>
+      </c>
+      <c r="I438" t="s">
+        <v>27</v>
+      </c>
+      <c r="J438" t="s">
         <v>2763</v>
       </c>
-      <c r="H438" s="1" t="n">
-        <v>41379</v>
-      </c>
-      <c r="I438" t="s">
-        <v>27</v>
-      </c>
-      <c r="J438" t="s">
+      <c r="K438" t="s">
         <v>2764</v>
       </c>
-      <c r="K438" t="s">
+      <c r="L438" t="s">
+        <v>47</v>
+      </c>
+      <c r="M438" t="s">
+        <v>241</v>
+      </c>
+      <c r="N438" t="s">
         <v>2765</v>
-      </c>
-      <c r="L438" t="s">
-        <v>30</v>
-      </c>
-      <c r="M438" t="s">
-        <v>31</v>
-      </c>
-      <c r="N438" t="s">
-        <v>32</v>
       </c>
       <c r="O438" t="s">
         <v>33</v>
@@ -44973,20 +44967,24 @@
       </c>
       <c r="R438"/>
       <c r="S438" t="b">
-        <v>0</v>
-      </c>
-      <c r="T438" s="1"/>
-      <c r="U438"/>
+        <v>1</v>
+      </c>
+      <c r="T438" s="1" t="n">
+        <v>28137</v>
+      </c>
+      <c r="U438" t="n">
+        <v>44</v>
+      </c>
     </row>
     <row r="439">
       <c r="A439" t="s">
         <v>2766</v>
       </c>
       <c r="B439" t="s">
-        <v>2747</v>
+        <v>2741</v>
       </c>
       <c r="C439" t="s">
-        <v>2748</v>
+        <v>2742</v>
       </c>
       <c r="D439" t="s">
         <v>2767</v>
@@ -44997,7 +44995,7 @@
         <v>2768</v>
       </c>
       <c r="H439" s="1" t="n">
-        <v>41295</v>
+        <v>41554</v>
       </c>
       <c r="I439" t="s">
         <v>27</v>
@@ -45012,10 +45010,10 @@
         <v>47</v>
       </c>
       <c r="M439" t="s">
-        <v>241</v>
+        <v>2771</v>
       </c>
       <c r="N439" t="s">
-        <v>2771</v>
+        <v>2772</v>
       </c>
       <c r="O439" t="s">
         <v>33</v>
@@ -45031,47 +45029,47 @@
         <v>1</v>
       </c>
       <c r="T439" s="1" t="n">
-        <v>28137</v>
+        <v>26281</v>
       </c>
       <c r="U439" t="n">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="s">
-        <v>2772</v>
+        <v>2773</v>
       </c>
       <c r="B440" t="s">
-        <v>2747</v>
+        <v>2741</v>
       </c>
       <c r="C440" t="s">
-        <v>2748</v>
+        <v>2742</v>
       </c>
       <c r="D440" t="s">
-        <v>2773</v>
+        <v>2774</v>
       </c>
       <c r="E440"/>
       <c r="F440"/>
       <c r="G440" t="s">
-        <v>2774</v>
+        <v>2775</v>
       </c>
       <c r="H440" s="1" t="n">
-        <v>41554</v>
+        <v>41852</v>
       </c>
       <c r="I440" t="s">
         <v>27</v>
       </c>
       <c r="J440" t="s">
-        <v>2775</v>
+        <v>2776</v>
       </c>
       <c r="K440" t="s">
-        <v>2776</v>
+        <v>2777</v>
       </c>
       <c r="L440" t="s">
         <v>47</v>
       </c>
       <c r="M440" t="s">
-        <v>2777</v>
+        <v>55</v>
       </c>
       <c r="N440" t="s">
         <v>2778</v>
@@ -45090,10 +45088,10 @@
         <v>1</v>
       </c>
       <c r="T440" s="1" t="n">
-        <v>26281</v>
+        <v>23605</v>
       </c>
       <c r="U440" t="n">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="441">
@@ -45101,10 +45099,10 @@
         <v>2779</v>
       </c>
       <c r="B441" t="s">
-        <v>2747</v>
+        <v>2741</v>
       </c>
       <c r="C441" t="s">
-        <v>2748</v>
+        <v>2742</v>
       </c>
       <c r="D441" t="s">
         <v>2780</v>
@@ -45115,7 +45113,7 @@
         <v>2781</v>
       </c>
       <c r="H441" s="1" t="n">
-        <v>41852</v>
+        <v>41834</v>
       </c>
       <c r="I441" t="s">
         <v>27</v>
@@ -45130,7 +45128,7 @@
         <v>47</v>
       </c>
       <c r="M441" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="N441" t="s">
         <v>2784</v>
@@ -45149,10 +45147,10 @@
         <v>1</v>
       </c>
       <c r="T441" s="1" t="n">
-        <v>23605</v>
+        <v>27609</v>
       </c>
       <c r="U441" t="n">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="442">
@@ -45160,10 +45158,10 @@
         <v>2785</v>
       </c>
       <c r="B442" t="s">
-        <v>2747</v>
+        <v>2741</v>
       </c>
       <c r="C442" t="s">
-        <v>2748</v>
+        <v>2742</v>
       </c>
       <c r="D442" t="s">
         <v>2786</v>
@@ -45174,7 +45172,7 @@
         <v>2787</v>
       </c>
       <c r="H442" s="1" t="n">
-        <v>41834</v>
+        <v>41837</v>
       </c>
       <c r="I442" t="s">
         <v>27</v>
@@ -45208,10 +45206,10 @@
         <v>1</v>
       </c>
       <c r="T442" s="1" t="n">
-        <v>27609</v>
+        <v>29689</v>
       </c>
       <c r="U442" t="n">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="443">
@@ -45219,10 +45217,10 @@
         <v>2791</v>
       </c>
       <c r="B443" t="s">
-        <v>2747</v>
+        <v>2741</v>
       </c>
       <c r="C443" t="s">
-        <v>2748</v>
+        <v>2742</v>
       </c>
       <c r="D443" t="s">
         <v>2792</v>
@@ -45233,7 +45231,7 @@
         <v>2793</v>
       </c>
       <c r="H443" s="1" t="n">
-        <v>41837</v>
+        <v>41339</v>
       </c>
       <c r="I443" t="s">
         <v>27</v>
@@ -45248,7 +45246,7 @@
         <v>47</v>
       </c>
       <c r="M443" t="s">
-        <v>32</v>
+        <v>241</v>
       </c>
       <c r="N443" t="s">
         <v>2796</v>
@@ -45267,10 +45265,10 @@
         <v>1</v>
       </c>
       <c r="T443" s="1" t="n">
-        <v>29689</v>
+        <v>24745</v>
       </c>
       <c r="U443" t="n">
-        <v>40</v>
+        <v>53</v>
       </c>
     </row>
     <row r="444">
@@ -45278,39 +45276,41 @@
         <v>2797</v>
       </c>
       <c r="B444" t="s">
-        <v>2747</v>
+        <v>2741</v>
       </c>
       <c r="C444" t="s">
-        <v>2748</v>
+        <v>2742</v>
       </c>
       <c r="D444" t="s">
         <v>2798</v>
       </c>
       <c r="E444"/>
-      <c r="F444"/>
+      <c r="F444" t="s">
+        <v>2799</v>
+      </c>
       <c r="G444" t="s">
-        <v>2799</v>
+        <v>2800</v>
       </c>
       <c r="H444" s="1" t="n">
-        <v>41339</v>
+        <v>41359</v>
       </c>
       <c r="I444" t="s">
         <v>27</v>
       </c>
       <c r="J444" t="s">
-        <v>2800</v>
+        <v>2801</v>
       </c>
       <c r="K444" t="s">
-        <v>2801</v>
+        <v>2802</v>
       </c>
       <c r="L444" t="s">
         <v>47</v>
       </c>
       <c r="M444" t="s">
-        <v>241</v>
+        <v>31</v>
       </c>
       <c r="N444" t="s">
-        <v>2802</v>
+        <v>32</v>
       </c>
       <c r="O444" t="s">
         <v>33</v>
@@ -45323,55 +45323,49 @@
       </c>
       <c r="R444"/>
       <c r="S444" t="b">
-        <v>1</v>
-      </c>
-      <c r="T444" s="1" t="n">
-        <v>24745</v>
-      </c>
-      <c r="U444" t="n">
-        <v>53</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T444" s="1"/>
+      <c r="U444"/>
     </row>
     <row r="445">
       <c r="A445" t="s">
         <v>2803</v>
       </c>
       <c r="B445" t="s">
-        <v>2747</v>
+        <v>2741</v>
       </c>
       <c r="C445" t="s">
-        <v>2748</v>
+        <v>2742</v>
       </c>
       <c r="D445" t="s">
         <v>2804</v>
       </c>
       <c r="E445"/>
-      <c r="F445" t="s">
+      <c r="F445"/>
+      <c r="G445" t="s">
         <v>2805</v>
       </c>
-      <c r="G445" t="s">
+      <c r="H445" s="1" t="n">
+        <v>41555</v>
+      </c>
+      <c r="I445" t="s">
+        <v>27</v>
+      </c>
+      <c r="J445" t="s">
         <v>2806</v>
       </c>
-      <c r="H445" s="1" t="n">
-        <v>41359</v>
-      </c>
-      <c r="I445" t="s">
-        <v>27</v>
-      </c>
-      <c r="J445" t="s">
+      <c r="K445" t="s">
         <v>2807</v>
-      </c>
-      <c r="K445" t="s">
-        <v>2808</v>
       </c>
       <c r="L445" t="s">
         <v>47</v>
       </c>
       <c r="M445" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="N445" t="s">
-        <v>32</v>
+        <v>2808</v>
       </c>
       <c r="O445" t="s">
         <v>33</v>
@@ -45384,31 +45378,37 @@
       </c>
       <c r="R445"/>
       <c r="S445" t="b">
-        <v>0</v>
-      </c>
-      <c r="T445" s="1"/>
-      <c r="U445"/>
+        <v>1</v>
+      </c>
+      <c r="T445" s="1" t="n">
+        <v>21999</v>
+      </c>
+      <c r="U445" t="n">
+        <v>61</v>
+      </c>
     </row>
     <row r="446">
       <c r="A446" t="s">
         <v>2809</v>
       </c>
       <c r="B446" t="s">
-        <v>2747</v>
+        <v>2741</v>
       </c>
       <c r="C446" t="s">
-        <v>2748</v>
+        <v>2742</v>
       </c>
       <c r="D446" t="s">
         <v>2810</v>
       </c>
       <c r="E446"/>
-      <c r="F446"/>
+      <c r="F446" t="s">
+        <v>66</v>
+      </c>
       <c r="G446" t="s">
         <v>2811</v>
       </c>
       <c r="H446" s="1" t="n">
-        <v>41555</v>
+        <v>40954</v>
       </c>
       <c r="I446" t="s">
         <v>27</v>
@@ -45423,7 +45423,7 @@
         <v>47</v>
       </c>
       <c r="M446" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="N446" t="s">
         <v>2814</v>
@@ -45442,10 +45442,10 @@
         <v>1</v>
       </c>
       <c r="T446" s="1" t="n">
-        <v>21999</v>
+        <v>27792</v>
       </c>
       <c r="U446" t="n">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="447">
@@ -45453,10 +45453,10 @@
         <v>2815</v>
       </c>
       <c r="B447" t="s">
-        <v>2747</v>
+        <v>2741</v>
       </c>
       <c r="C447" t="s">
-        <v>2748</v>
+        <v>2742</v>
       </c>
       <c r="D447" t="s">
         <v>2816</v>
@@ -45510,10 +45510,10 @@
         <v>2821</v>
       </c>
       <c r="B448" t="s">
-        <v>2747</v>
+        <v>2741</v>
       </c>
       <c r="C448" t="s">
-        <v>2748</v>
+        <v>2742</v>
       </c>
       <c r="D448" t="s">
         <v>2822</v>
@@ -45567,10 +45567,10 @@
         <v>2827</v>
       </c>
       <c r="B449" t="s">
-        <v>2747</v>
+        <v>2741</v>
       </c>
       <c r="C449" t="s">
-        <v>2748</v>
+        <v>2742</v>
       </c>
       <c r="D449" t="s">
         <v>2828</v>
@@ -48377,7 +48377,7 @@
         <v>23623</v>
       </c>
       <c r="U496" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="497">
@@ -53741,7 +53741,7 @@
         <v>21071</v>
       </c>
       <c r="U588" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="589">
@@ -54333,7 +54333,7 @@
         <v>27643</v>
       </c>
       <c r="U598" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="599">
@@ -56909,7 +56909,7 @@
       </c>
       <c r="E643"/>
       <c r="F643" t="s">
-        <v>2652</v>
+        <v>2646</v>
       </c>
       <c r="G643" t="s">
         <v>4001</v>
@@ -57249,7 +57249,7 @@
         <v>23625</v>
       </c>
       <c r="U648" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="649">
@@ -62200,7 +62200,7 @@
       </c>
       <c r="E734"/>
       <c r="F734" t="s">
-        <v>2805</v>
+        <v>2799</v>
       </c>
       <c r="G734" t="s">
         <v>4542</v>
@@ -65055,7 +65055,7 @@
       </c>
       <c r="E783"/>
       <c r="F783" t="s">
-        <v>2762</v>
+        <v>2756</v>
       </c>
       <c r="G783" t="s">
         <v>4838</v>
@@ -65289,7 +65289,7 @@
       </c>
       <c r="E787"/>
       <c r="F787" t="s">
-        <v>2646</v>
+        <v>2640</v>
       </c>
       <c r="G787" t="s">
         <v>4861</v>
@@ -65574,7 +65574,7 @@
       </c>
       <c r="E792"/>
       <c r="F792" t="s">
-        <v>2627</v>
+        <v>2621</v>
       </c>
       <c r="G792" t="s">
         <v>4888</v>
@@ -67853,7 +67853,7 @@
         <v>24717</v>
       </c>
       <c r="U830" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="831">
@@ -71614,7 +71614,7 @@
         <v>29101</v>
       </c>
       <c r="U895" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="896">
@@ -74638,7 +74638,7 @@
         <v>47</v>
       </c>
       <c r="M947" t="s">
-        <v>2666</v>
+        <v>2660</v>
       </c>
       <c r="N947" t="s">
         <v>5843</v>
@@ -75297,7 +75297,7 @@
         <v>25453</v>
       </c>
       <c r="U958" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="959">
@@ -75966,7 +75966,7 @@
         <v>32</v>
       </c>
       <c r="N970" t="s">
-        <v>2739</v>
+        <v>2733</v>
       </c>
       <c r="O970" t="s">
         <v>33</v>
@@ -77735,7 +77735,7 @@
         <v>24720</v>
       </c>
       <c r="U1000" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="1001">

</xml_diff>

<commit_message>
ajustes após reinstalação do monterey - momento que voltou a funcionar.
</commit_message>
<xml_diff>
--- a/report/acs.xlsx
+++ b/report/acs.xlsx
@@ -22442,7 +22442,7 @@
         <v>29165</v>
       </c>
       <c r="U58" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59">
@@ -22733,7 +22733,7 @@
         <v>21861</v>
       </c>
       <c r="U63" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64">
@@ -24786,7 +24786,7 @@
         <v>32089</v>
       </c>
       <c r="U98" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="99">
@@ -29379,7 +29379,7 @@
         <v>25881</v>
       </c>
       <c r="U177" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="178">
@@ -30669,7 +30669,7 @@
         <v>20400</v>
       </c>
       <c r="U199" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="200">
@@ -37069,7 +37069,7 @@
         <v>33552</v>
       </c>
       <c r="U309" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="310">
@@ -47528,7 +47528,7 @@
         <v>28438</v>
       </c>
       <c r="U488" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="489">
@@ -48118,7 +48118,7 @@
         <v>31360</v>
       </c>
       <c r="U498" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="499">
@@ -53421,7 +53421,7 @@
         <v>32455</v>
       </c>
       <c r="U589" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="590">
@@ -64530,7 +64530,7 @@
         <v>29900</v>
       </c>
       <c r="U780" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="781">

</xml_diff>